<commit_message>
GDE-9324 - added other deals
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/New_UAT_Deals_Dataset_Masterlist.xlsx
+++ b/DataSet/NewUATDeals_DataSet/New_UAT_Deals_Dataset_Masterlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E5E44A-E9A0-4A99-82D2-B8ACFEB46508}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339C8BC0-1BA0-4BC4-AE35-A22244880A71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3120" windowWidth="28800" windowHeight="7830" xr2:uid="{2A7F3597-B565-48CF-83A4-3B0A861071F2}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="28800" windowHeight="7830" xr2:uid="{2A7F3597-B565-48CF-83A4-3B0A861071F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>rowid</t>
   </si>
@@ -57,13 +57,49 @@
   </si>
   <si>
     <t>\DataSet\NewUATDeals_DataSet\</t>
+  </si>
+  <si>
+    <t>Deal_CH_EDU_BILAT.xlsx</t>
+  </si>
+  <si>
+    <t>Deal_LBT_BILAT.xlsx</t>
+  </si>
+  <si>
+    <t>Deal_New_Life_BILAT.xlsx</t>
+  </si>
+  <si>
+    <t>Deal_PIM_Future_BILAT.xlsx</t>
+  </si>
+  <si>
+    <t>LBT_BILAT</t>
+  </si>
+  <si>
+    <t>New_Life_BILAT</t>
+  </si>
+  <si>
+    <t>PIM_Future_BILAT</t>
+  </si>
+  <si>
+    <t>CH_EDU_BILAT</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +118,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -435,15 +477,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063B01CE-A5EA-49EA-8307-90742B6C5656}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -476,7 +518,64 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GDE-9324 - addressed comments
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/New_UAT_Deals_Dataset_Masterlist.xlsx
+++ b/DataSet/NewUATDeals_DataSet/New_UAT_Deals_Dataset_Masterlist.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339C8BC0-1BA0-4BC4-AE35-A22244880A71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DF563C-B9BD-4E89-AF86-8865082A4ACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="390" windowWidth="28800" windowHeight="7830" xr2:uid="{2A7F3597-B565-48CF-83A4-3B0A861071F2}"/>
+    <workbookView xWindow="-1875" yWindow="5415" windowWidth="28800" windowHeight="7830" xr2:uid="{2A7F3597-B565-48CF-83A4-3B0A861071F2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Clients" sheetId="1" r:id="rId1"/>
+    <sheet name="UAT_Deal_Scenarios" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,9 +41,6 @@
     <t>Path</t>
   </si>
   <si>
-    <t>UAT_Client</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>UAT_Deal_Scenario_Name</t>
   </si>
 </sst>
 </file>
@@ -480,12 +480,12 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -495,83 +495,83 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDE-9497: Initial Commit for Quick Party of PT Health
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/New_UAT_Deals_Dataset_Masterlist.xlsx
+++ b/DataSet/NewUATDeals_DataSet/New_UAT_Deals_Dataset_Masterlist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DF563C-B9BD-4E89-AF86-8865082A4ACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BD0E9F-D5EC-4A6B-9B4C-726ED4D181B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1875" yWindow="5415" windowWidth="28800" windowHeight="7830" xr2:uid="{2A7F3597-B565-48CF-83A4-3B0A861071F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2A7F3597-B565-48CF-83A4-3B0A861071F2}"/>
   </bookViews>
   <sheets>
     <sheet name="UAT_Deal_Scenarios" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>rowid</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>UAT_Deal_Scenario_Name</t>
+  </si>
+  <si>
+    <t>PT_Health_SYND</t>
+  </si>
+  <si>
+    <t>Deal_PT_Health_Syndicated.xlsx</t>
   </si>
 </sst>
 </file>
@@ -156,12 +162,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -477,20 +486,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063B01CE-A5EA-49EA-8307-90742B6C5656}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,7 +513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -518,7 +527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -532,7 +541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -546,7 +555,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -560,7 +569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -572,6 +581,20 @@
       </c>
       <c r="D6" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>